<commit_message>
Corrigido uns bugs de posição do mouse e colocado um tutorial de como usar o pyinstaller
</commit_message>
<xml_diff>
--- a/dist/xlsx/emprestimo.xlsx
+++ b/dist/xlsx/emprestimo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://animaeducacao.sharepoint.com/sites/NSIUnisulG.Florianpolis/Documentos Compartilhados/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="84" documentId="13_ncr:1_{20142758-98EB-4B46-A8F1-B8EB3D882068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{624F574A-9408-4E1D-A748-9432187E9D00}"/>
+  <xr:revisionPtr revIDLastSave="146" documentId="13_ncr:1_{20142758-98EB-4B46-A8F1-B8EB3D882068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8160E42C-A896-47A9-866C-8E359A27F856}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{134297C1-7B4C-4C6C-8CB9-91DF777EEECD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Equipamento</t>
   </si>
@@ -47,6 +47,12 @@
     <t>Data</t>
   </si>
   <si>
+    <t>Tecnico</t>
+  </si>
+  <si>
+    <t>Responsavel</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -62,13 +68,13 @@
     <t>Audi C</t>
   </si>
   <si>
-    <t>Responsavel</t>
+    <t>Kauan</t>
   </si>
   <si>
     <t>Laura Roin</t>
   </si>
   <si>
-    <t>Kauan</t>
+    <t>Entregue</t>
   </si>
   <si>
     <t>Pointer e Micro</t>
@@ -80,12 +86,6 @@
     <t>Eloisa</t>
   </si>
   <si>
-    <t>Não Entregue</t>
-  </si>
-  <si>
-    <t>Entregue</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Entregue</t>
   </si>
   <si>
@@ -101,16 +101,13 @@
     <t>Habilidades 1</t>
   </si>
   <si>
-    <t>Poniter</t>
-  </si>
-  <si>
     <t>114D</t>
   </si>
   <si>
     <t>Eliane</t>
   </si>
   <si>
-    <t>Tecnico</t>
+    <t xml:space="preserve">Entregue </t>
   </si>
   <si>
     <t>ADAPTADOR DE REDE</t>
@@ -147,13 +144,49 @@
   </si>
   <si>
     <t>Eliane Fraevert</t>
+  </si>
+  <si>
+    <t>Notebook Vaio</t>
+  </si>
+  <si>
+    <t>Extra Aula</t>
+  </si>
+  <si>
+    <t>Aluna</t>
+  </si>
+  <si>
+    <t>219B</t>
+  </si>
+  <si>
+    <t>Prof</t>
+  </si>
+  <si>
+    <t>316D</t>
+  </si>
+  <si>
+    <t>Thaise Gerber</t>
+  </si>
+  <si>
+    <t>Não entregue</t>
+  </si>
+  <si>
+    <t>211H</t>
+  </si>
+  <si>
+    <t>Nathalia (48 999467019)</t>
+  </si>
+  <si>
+    <t>318D</t>
+  </si>
+  <si>
+    <t>Jurema (48 99962-9662)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +219,13 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -229,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -252,6 +292,9 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,10 +310,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -593,14 +632,14 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -609,7 +648,7 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="26.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -620,27 +659,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="5">
         <v>45551</v>
@@ -649,18 +688,18 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="5">
         <v>45552</v>
@@ -669,13 +708,13 @@
         <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -692,15 +731,15 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="C5" s="5">
         <v>45553</v>
@@ -709,18 +748,18 @@
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C6" s="5">
         <v>45555</v>
@@ -729,18 +768,18 @@
         <v>19</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5">
         <v>45559</v>
@@ -749,18 +788,18 @@
         <v>10</v>
       </c>
       <c r="E7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="C8" s="5">
         <v>45459</v>
@@ -769,18 +808,18 @@
         <v>10</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="C9" s="5">
         <v>45561</v>
@@ -789,18 +828,18 @@
         <v>10</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5">
         <v>45522</v>
@@ -809,69 +848,153 @@
         <v>19</v>
       </c>
       <c r="E10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="5">
+        <v>45565</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="5">
+        <v>45566</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="5">
+        <v>45566</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="5">
+        <v>45568</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="5">
+        <v>45573</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="5">
+        <v>45581</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="5">
+        <v>45581</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="5"/>
@@ -879,7 +1002,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="5"/>
@@ -887,7 +1010,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="5"/>
@@ -895,7 +1018,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="5"/>
@@ -911,15 +1034,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="df29e128-5ec9-41e9-af68-5f97b1a2cc5a">
@@ -930,6 +1044,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1179,47 +1302,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1613DD64-3346-4DD5-8616-B482126BEF27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3FE17C1-AA90-47A0-BFF0-D3E9C0437ABC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3FE17C1-AA90-47A0-BFF0-D3E9C0437ABC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="df29e128-5ec9-41e9-af68-5f97b1a2cc5a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4d588f8c-4f45-47ca-b7bd-9cffca7f8789"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1613DD64-3346-4DD5-8616-B482126BEF27}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A59C653-3479-4480-890A-8D2145B093BB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="df29e128-5ec9-41e9-af68-5f97b1a2cc5a"/>
-    <ds:schemaRef ds:uri="4d588f8c-4f45-47ca-b7bd-9cffca7f8789"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A59C653-3479-4480-890A-8D2145B093BB}"/>
 </file>
</xml_diff>